<commit_message>
sistema colores aprender automatico con traductor
</commit_message>
<xml_diff>
--- a/src/lista.xlsx
+++ b/src/lista.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abces\Desktop\idiomaEN\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4316421B-F354-406D-8756-199BE2946B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF3D85-0A0D-4A28-96D2-1253A4547F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="colores" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="146">
   <si>
     <t>SETTINGS</t>
   </si>
@@ -94,6 +95,375 @@
   </si>
   <si>
     <t>System</t>
+  </si>
+  <si>
+    <t>Colores más comunes</t>
+  </si>
+  <si>
+    <t>Traducción</t>
+  </si>
+  <si>
+    <t>Aqua/Cyan</t>
+  </si>
+  <si>
+    <t>Agua/Cian</t>
+  </si>
+  <si>
+    <t>Aquamarina</t>
+  </si>
+  <si>
+    <t>Aguamarina</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Azur</t>
+  </si>
+  <si>
+    <t>Beige</t>
+  </si>
+  <si>
+    <t>Castaño claro</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Negro</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Café</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Coral</t>
+  </si>
+  <si>
+    <t>Crimson</t>
+  </si>
+  <si>
+    <t>Carmesí</t>
+  </si>
+  <si>
+    <t>Dark gray </t>
+  </si>
+  <si>
+    <t>Gris oscuro</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Oro</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Gris</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>Indigo</t>
+  </si>
+  <si>
+    <t>Índigo</t>
+  </si>
+  <si>
+    <t>Ivory</t>
+  </si>
+  <si>
+    <t>Marfil</t>
+  </si>
+  <si>
+    <t>Lavender</t>
+  </si>
+  <si>
+    <t>Lavanda</t>
+  </si>
+  <si>
+    <t>Light gray</t>
+  </si>
+  <si>
+    <t>Gris claro</t>
+  </si>
+  <si>
+    <t>Magenta</t>
+  </si>
+  <si>
+    <t>Maroon</t>
+  </si>
+  <si>
+    <t>Granate</t>
+  </si>
+  <si>
+    <t>Misty Rose</t>
+  </si>
+  <si>
+    <t>Rosa brumoso</t>
+  </si>
+  <si>
+    <t>Navy </t>
+  </si>
+  <si>
+    <t>Azul Marino</t>
+  </si>
+  <si>
+    <t>Olive</t>
+  </si>
+  <si>
+    <t>Oliva</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Naranja</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>Plum</t>
+  </si>
+  <si>
+    <t>Ciruela</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Morado</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Rojo</t>
+  </si>
+  <si>
+    <t>Salmon</t>
+  </si>
+  <si>
+    <t>Salmón</t>
+  </si>
+  <si>
+    <t>Silver </t>
+  </si>
+  <si>
+    <t>Plateado</t>
+  </si>
+  <si>
+    <t>Sky</t>
+  </si>
+  <si>
+    <t>Cielo</t>
+  </si>
+  <si>
+    <t>Tan </t>
+  </si>
+  <si>
+    <t>Canela</t>
+  </si>
+  <si>
+    <t>Teal </t>
+  </si>
+  <si>
+    <t>Verde azulado</t>
+  </si>
+  <si>
+    <t>Turquoise </t>
+  </si>
+  <si>
+    <t>Turquesa</t>
+  </si>
+  <si>
+    <t>White </t>
+  </si>
+  <si>
+    <t>Blanco</t>
+  </si>
+  <si>
+    <t>White smoke </t>
+  </si>
+  <si>
+    <t>Humo</t>
+  </si>
+  <si>
+    <t>Yellow </t>
+  </si>
+  <si>
+    <t>Amarillo</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>English Phrase</t>
+  </si>
+  <si>
+    <t>The sky is a clear aqua.</t>
+  </si>
+  <si>
+    <t>Aquamarine</t>
+  </si>
+  <si>
+    <t>The ocean is a beautiful aquamarine.</t>
+  </si>
+  <si>
+    <t>The azure sky is so clear.</t>
+  </si>
+  <si>
+    <t>The sand is soft and beige.</t>
+  </si>
+  <si>
+    <t>The night sky is dark black.</t>
+  </si>
+  <si>
+    <t>The ocean is deep blue.</t>
+  </si>
+  <si>
+    <t>The tree trunk is brown.</t>
+  </si>
+  <si>
+    <t>The cake is dark chocolate.</t>
+  </si>
+  <si>
+    <t>The coral reef is colorful.</t>
+  </si>
+  <si>
+    <t>The rose is a deep crimson.</t>
+  </si>
+  <si>
+    <t>Dark Gray</t>
+  </si>
+  <si>
+    <t>The clouds are dark gray.</t>
+  </si>
+  <si>
+    <t>The sun is shining gold.</t>
+  </si>
+  <si>
+    <t>The rock is gray and old.</t>
+  </si>
+  <si>
+    <t>The grass is so green.</t>
+  </si>
+  <si>
+    <t>The flower is a bright indigo.</t>
+  </si>
+  <si>
+    <t>The dress is a soft ivory.</t>
+  </si>
+  <si>
+    <t>The field of lavender is purple.</t>
+  </si>
+  <si>
+    <t>Light Gray</t>
+  </si>
+  <si>
+    <t>The clouds are light gray.</t>
+  </si>
+  <si>
+    <t>The flower is a bright magenta.</t>
+  </si>
+  <si>
+    <t>The carpet is a deep maroon.</t>
+  </si>
+  <si>
+    <t>The sky is a misty rose.</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>The sailor's uniform is navy blue.</t>
+  </si>
+  <si>
+    <t>The olive oil is green.</t>
+  </si>
+  <si>
+    <t>The orange is so juicy.</t>
+  </si>
+  <si>
+    <t>The cotton candy is pink.</t>
+  </si>
+  <si>
+    <t>The plum is dark purple.</t>
+  </si>
+  <si>
+    <t>The grape is dark purple.</t>
+  </si>
+  <si>
+    <t>The apple is bright red.</t>
+  </si>
+  <si>
+    <t>The fish is pink salmon.</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>The moon is shining silver.</t>
+  </si>
+  <si>
+    <t>The sky is a clear blue.</t>
+  </si>
+  <si>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t>The leather is a light brown.</t>
+  </si>
+  <si>
+    <t>Teal</t>
+  </si>
+  <si>
+    <t>The duck is a bright teal.</t>
+  </si>
+  <si>
+    <t>Turquoise</t>
+  </si>
+  <si>
+    <t>The water is a bright turquoise.</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>The snow is pure white.</t>
+  </si>
+  <si>
+    <t>White Smoke</t>
+  </si>
+  <si>
+    <t>The smoke is white and wispy.</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>The lemon is bright yellow.</t>
   </si>
 </sst>
 </file>
@@ -413,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection sqref="A1:B23"/>
     </sheetView>
   </sheetViews>
@@ -611,4 +981,667 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECECF02-B9E8-485B-9666-649A80F244AB}">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
el sitema no tiene traductor automatico, por que puede que el traductor no este bien, todo esta en la base de datos, si es automatico la voz
</commit_message>
<xml_diff>
--- a/src/lista.xlsx
+++ b/src/lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abces\Desktop\idiomaEN\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF3D85-0A0D-4A28-96D2-1253A4547F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695CE251-A357-4DE7-81CC-0673F6C75051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="174">
   <si>
     <t>SETTINGS</t>
   </si>
@@ -97,54 +97,24 @@
     <t>System</t>
   </si>
   <si>
-    <t>Colores más comunes</t>
-  </si>
-  <si>
-    <t>Traducción</t>
-  </si>
-  <si>
     <t>Aqua/Cyan</t>
   </si>
   <si>
-    <t>Agua/Cian</t>
-  </si>
-  <si>
-    <t>Aquamarina</t>
-  </si>
-  <si>
-    <t>Aguamarina</t>
-  </si>
-  <si>
     <t>Azure</t>
   </si>
   <si>
-    <t>Azur</t>
-  </si>
-  <si>
     <t>Beige</t>
   </si>
   <si>
-    <t>Castaño claro</t>
-  </si>
-  <si>
     <t>Black</t>
   </si>
   <si>
-    <t>Negro</t>
-  </si>
-  <si>
     <t>Blue</t>
   </si>
   <si>
-    <t>Azul</t>
-  </si>
-  <si>
     <t>Brown</t>
   </si>
   <si>
-    <t>Café</t>
-  </si>
-  <si>
     <t>Chocolate</t>
   </si>
   <si>
@@ -154,174 +124,60 @@
     <t>Crimson</t>
   </si>
   <si>
-    <t>Carmesí</t>
-  </si>
-  <si>
-    <t>Dark gray </t>
-  </si>
-  <si>
-    <t>Gris oscuro</t>
-  </si>
-  <si>
     <t>Gold</t>
   </si>
   <si>
-    <t>Oro</t>
-  </si>
-  <si>
     <t>Gray</t>
   </si>
   <si>
-    <t>Gris</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
-    <t>Verde</t>
-  </si>
-  <si>
     <t>Indigo</t>
   </si>
   <si>
-    <t>Índigo</t>
-  </si>
-  <si>
     <t>Ivory</t>
   </si>
   <si>
-    <t>Marfil</t>
-  </si>
-  <si>
     <t>Lavender</t>
   </si>
   <si>
-    <t>Lavanda</t>
-  </si>
-  <si>
-    <t>Light gray</t>
-  </si>
-  <si>
-    <t>Gris claro</t>
-  </si>
-  <si>
     <t>Magenta</t>
   </si>
   <si>
     <t>Maroon</t>
   </si>
   <si>
-    <t>Granate</t>
-  </si>
-  <si>
     <t>Misty Rose</t>
   </si>
   <si>
-    <t>Rosa brumoso</t>
-  </si>
-  <si>
-    <t>Navy </t>
-  </si>
-  <si>
-    <t>Azul Marino</t>
-  </si>
-  <si>
     <t>Olive</t>
   </si>
   <si>
-    <t>Oliva</t>
-  </si>
-  <si>
     <t>Orange</t>
   </si>
   <si>
-    <t>Naranja</t>
-  </si>
-  <si>
     <t>Pink</t>
   </si>
   <si>
-    <t>Rosa</t>
-  </si>
-  <si>
     <t>Plum</t>
   </si>
   <si>
-    <t>Ciruela</t>
-  </si>
-  <si>
     <t>Purple</t>
   </si>
   <si>
-    <t>Morado</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
-    <t>Rojo</t>
-  </si>
-  <si>
     <t>Salmon</t>
   </si>
   <si>
-    <t>Salmón</t>
-  </si>
-  <si>
-    <t>Silver </t>
-  </si>
-  <si>
-    <t>Plateado</t>
-  </si>
-  <si>
     <t>Sky</t>
   </si>
   <si>
-    <t>Cielo</t>
-  </si>
-  <si>
-    <t>Tan </t>
-  </si>
-  <si>
-    <t>Canela</t>
-  </si>
-  <si>
-    <t>Teal </t>
-  </si>
-  <si>
-    <t>Verde azulado</t>
-  </si>
-  <si>
-    <t>Turquoise </t>
-  </si>
-  <si>
-    <t>Turquesa</t>
-  </si>
-  <si>
-    <t>White </t>
-  </si>
-  <si>
-    <t>Blanco</t>
-  </si>
-  <si>
-    <t>White smoke </t>
-  </si>
-  <si>
-    <t>Humo</t>
-  </si>
-  <si>
-    <t>Yellow </t>
-  </si>
-  <si>
-    <t>Amarillo</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
-    <t>English Phrase</t>
-  </si>
-  <si>
     <t>The sky is a clear aqua.</t>
   </si>
   <si>
@@ -464,6 +320,234 @@
   </si>
   <si>
     <t>The lemon is bright yellow.</t>
+  </si>
+  <si>
+    <t>Frase en Inglés</t>
+  </si>
+  <si>
+    <t>Traducción al Español</t>
+  </si>
+  <si>
+    <t>Explicación</t>
+  </si>
+  <si>
+    <t>El cielo es de un azul claro.</t>
+  </si>
+  <si>
+    <t>Aqua es una forma más poética de decir "azul claro".</t>
+  </si>
+  <si>
+    <t>El océano es de un hermoso color aguamarina.</t>
+  </si>
+  <si>
+    <t>Aquamarine es un tono de azul verdoso, similar al color del mar.</t>
+  </si>
+  <si>
+    <t>El cielo azur es tan claro.</t>
+  </si>
+  <si>
+    <t>Azure es otro sinónimo de "azul cielo", pero con una connotación más poética.</t>
+  </si>
+  <si>
+    <t>La arena es suave y beige.</t>
+  </si>
+  <si>
+    <t>Beige es un color entre el crema y el marrón claro.</t>
+  </si>
+  <si>
+    <t>El cielo nocturno es negro oscuro.</t>
+  </si>
+  <si>
+    <t>Una forma sencilla de describir el color del cielo en la noche.</t>
+  </si>
+  <si>
+    <t>El océano es azul profundo.</t>
+  </si>
+  <si>
+    <t>Deep blue enfatiza la intensidad del color azul del océano.</t>
+  </si>
+  <si>
+    <t>El tronco del árbol es marrón.</t>
+  </si>
+  <si>
+    <t>Un color común para los troncos de los árboles.</t>
+  </si>
+  <si>
+    <t>El pastel es de chocolate oscuro.</t>
+  </si>
+  <si>
+    <t>Un sabor y color común para los pasteles.</t>
+  </si>
+  <si>
+    <t>El arrecife de coral es colorido.</t>
+  </si>
+  <si>
+    <t>Los arrecifes de coral son conocidos por su gran variedad de colores.</t>
+  </si>
+  <si>
+    <t>La rosa es de un rojo carmesí intenso.</t>
+  </si>
+  <si>
+    <t>Crimson es un tono de rojo muy intenso y oscuro.</t>
+  </si>
+  <si>
+    <t>Las nubes son de un gris oscuro.</t>
+  </si>
+  <si>
+    <t>Un color común para las nubes antes de una tormenta.</t>
+  </si>
+  <si>
+    <t>El sol brilla dorado.</t>
+  </si>
+  <si>
+    <t>Una descripción poética del color del sol.</t>
+  </si>
+  <si>
+    <t>La roca es gris y vieja.</t>
+  </si>
+  <si>
+    <t>Un color común para las rocas y las piedras.</t>
+  </si>
+  <si>
+    <t>La hierba está muy verde.</t>
+  </si>
+  <si>
+    <t>Un color asociado con la naturaleza y la vida.</t>
+  </si>
+  <si>
+    <t>La flor es de un color índigo brillante.</t>
+  </si>
+  <si>
+    <t>Indigo es un tono de azul oscuro, casi morado.</t>
+  </si>
+  <si>
+    <t>El vestido es de un suave color marfil.</t>
+  </si>
+  <si>
+    <t>Ivory es un color blanco cremoso, a menudo asociado con la elegancia.</t>
+  </si>
+  <si>
+    <t>El campo de lavanda es morado.</t>
+  </si>
+  <si>
+    <t>Lavender es un tono de morado pálido y suave.</t>
+  </si>
+  <si>
+    <t>Las nubes son de un gris claro.</t>
+  </si>
+  <si>
+    <t>Un color común para las nubes en un día nublado.</t>
+  </si>
+  <si>
+    <t>La flor es de un color magenta brillante.</t>
+  </si>
+  <si>
+    <t>Magenta es un tono de rosa muy intenso y vibrante.</t>
+  </si>
+  <si>
+    <t>La alfombra es de un color burdeos intenso.</t>
+  </si>
+  <si>
+    <t>Maroon es un tono de rojo oscuro, casi marrón.</t>
+  </si>
+  <si>
+    <t>El cielo es de un rosa pálido.</t>
+  </si>
+  <si>
+    <t>Misty rose es un tono de rosa muy suave y delicado.</t>
+  </si>
+  <si>
+    <t>El uniforme de marinero es azul marino.</t>
+  </si>
+  <si>
+    <t>Navy blue es un tono de azul oscuro, asociado con la marina.</t>
+  </si>
+  <si>
+    <t>El aceite de oliva es verde.</t>
+  </si>
+  <si>
+    <t>El aceite de oliva virgen extra tiene un color verde.</t>
+  </si>
+  <si>
+    <t>La naranja está muy jugosa.</t>
+  </si>
+  <si>
+    <t>Un color y sabor asociados con la fruta.</t>
+  </si>
+  <si>
+    <t>El algodón de azúcar es rosa.</t>
+  </si>
+  <si>
+    <t>Un color asociado con la dulzura y la infancia.</t>
+  </si>
+  <si>
+    <t>La ciruela es de color morado oscuro.</t>
+  </si>
+  <si>
+    <t>Un color asociado con la fruta.</t>
+  </si>
+  <si>
+    <t>La uva es de color morado oscuro.</t>
+  </si>
+  <si>
+    <t>Un color común para las uvas.</t>
+  </si>
+  <si>
+    <t>La manzana es de un rojo brillante.</t>
+  </si>
+  <si>
+    <t>Un color asociado con la fruta y la energía.</t>
+  </si>
+  <si>
+    <t>El pescado es salmón rosado.</t>
+  </si>
+  <si>
+    <t>Un tipo de pescado conocido por su color rosado.</t>
+  </si>
+  <si>
+    <t>La luna brilla plateada.</t>
+  </si>
+  <si>
+    <t>Una descripción poética del color de la luna.</t>
+  </si>
+  <si>
+    <t>Una forma sencilla de describir el color del cielo.</t>
+  </si>
+  <si>
+    <t>El cuero es de un marrón claro.</t>
+  </si>
+  <si>
+    <t>Un color común para el cuero.</t>
+  </si>
+  <si>
+    <t>El pato es de un color azul verdoso brillante.</t>
+  </si>
+  <si>
+    <t>Teal es un tono de azul verdoso, similar al color del agua.</t>
+  </si>
+  <si>
+    <t>El agua es de un color turquesa brillante.</t>
+  </si>
+  <si>
+    <t>Turquoise es un tono de azul verdoso, asociado con el agua.</t>
+  </si>
+  <si>
+    <t>La nieve es blanca pura.</t>
+  </si>
+  <si>
+    <t>Un color asociado con la pureza y el invierno.</t>
+  </si>
+  <si>
+    <t>El humo es blanco y tenue.</t>
+  </si>
+  <si>
+    <t>Una descripción del humo blanco.</t>
+  </si>
+  <si>
+    <t>El limón es de un amarillo brillante.</t>
+  </si>
+  <si>
+    <t>Un color asociado con la fruta y el sol.</t>
   </si>
 </sst>
 </file>
@@ -987,28 +1071,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECECF02-B9E8-485B-9666-649A80F244AB}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="30.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1016,16 +1101,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1033,16 +1118,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,16 +1135,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,16 +1152,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1084,16 +1169,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1101,16 +1186,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1118,16 +1203,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1135,16 +1220,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1152,16 +1237,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1169,16 +1254,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1186,16 +1271,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,16 +1288,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1220,16 +1305,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1237,16 +1322,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1254,16 +1339,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1271,16 +1356,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1288,16 +1373,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1305,16 +1390,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1322,16 +1407,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1339,16 +1424,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="E21" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1356,16 +1441,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1373,16 +1458,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1390,16 +1475,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1407,16 +1492,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="E25" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,16 +1509,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="E26" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1441,16 +1526,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1458,16 +1543,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1475,16 +1560,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1492,16 +1577,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>157</v>
       </c>
       <c r="E30" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1509,16 +1594,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1526,16 +1611,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1543,16 +1628,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1560,16 +1645,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="E34" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,16 +1662,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="E35" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,16 +1679,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1611,16 +1696,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="E37" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1628,16 +1713,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>